<commit_message>
Updating hc_cond with new CCSR codes and adding BODY systems
</commit_message>
<xml_diff>
--- a/dictionaries/stat_labels.xlsx
+++ b/dictionaries/stat_labels.xlsx
@@ -1,29 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily.mitchell\OneDrive - HHS Office of the Secretary\Desktop\GitHub\hhs_ahrq\MEPS-tables\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EE1A38-B2C5-4971-9E2F-DC9CDE4B7B2C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59C76CA-1FD3-4D33-9554-81BB61FB69B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11775" yWindow="480" windowWidth="15525" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29745" yWindow="1200" windowWidth="19815" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sig_digits" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sig_digits!$A$1:$F$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sig_digits!$A$1:$I$19</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t>table_series</t>
   </si>
@@ -146,13 +159,22 @@
   </si>
   <si>
     <t>hc_cond_icd10</t>
+  </si>
+  <si>
+    <t>rnd_digits</t>
+  </si>
+  <si>
+    <t>se_digits</t>
+  </si>
+  <si>
+    <t>order</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,6 +305,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -629,9 +657,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -987,378 +1017,559 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:A15"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1000</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1000</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>32</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1000</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1000</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F7">
+        <v>0.01</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>1000000</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>25</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>33</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>1000</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>33</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>1000</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E16">
+      <c r="F16" s="2">
         <v>1000000</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>35</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>37</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>1000</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>31</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>16</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>28</v>
       </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E19">
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F24" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I19" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I19">
+      <sortCondition ref="A1:A19"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>